<commit_message>
removed path prefix from ms method
</commit_message>
<xml_diff>
--- a/agilent_methods/experimentTemplate.xlsx
+++ b/agilent_methods/experimentTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gkreder/RapidSky/agilent_methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C9C99F-5187-844A-B384-C58A713F81A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F434B802-2AFE-F746-A618-415685DF5BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
@@ -374,10 +374,10 @@
     <t>Reequilibrate</t>
   </si>
   <si>
-    <t>D:\Projects\Default\Methods\2023-03-02_dodd_4Bit_POS.m</t>
-  </si>
-  <si>
-    <t>D:\Projects\Default\Methods\2023-03-02_dodd_4Bit_NEG.m</t>
+    <t>2023-03-02_dodd_4Bit_POS.m</t>
+  </si>
+  <si>
+    <t>2023-03-02_dodd_4Bit_NEG.m</t>
   </si>
 </sst>
 </file>
@@ -1227,41 +1227,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4813,8 +4821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>